<commit_message>
add mrdodo and toringo scoring systems
</commit_message>
<xml_diff>
--- a/to-do.xlsx
+++ b/to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\My Drive (matteopardi2@gmail.com)\Projects\TENNIS - Tennis-Ranking (branch v2.0)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428392C9-43FC-446E-82F7-1F2BF2AA70D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257D7223-7DCD-4F6E-9508-C868048A5255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9915" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="to-do" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,51 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>Fai LogLikelihoodTerm.py</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>Fai Loss.py</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>Fai TennisDataframe.py</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>Intendo la classe derivata da pd.Dataframe… con le colonne già inizializzate</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>Fai import_notion_csv.py</t>
+  </si>
+  <si>
+    <t>e genera il tennis dataframe</t>
+  </si>
+  <si>
+    <t>in ingresso prende un tennis dataframe</t>
+  </si>
+  <si>
+    <t>Fai TennisUniverse.py, escluso il metodo di ottimizzazione</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>Fai il metodo di ottimizzazione di TennisUniverse</t>
   </si>
 </sst>
 </file>
@@ -141,7 +186,187 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -211,8 +436,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
-  <autoFilter ref="A1:I5" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}" name="Table1" displayName="Table1" ref="A1:I11" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21">
+  <autoFilter ref="A1:I11" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4C27F59C-46C4-4AF8-8CE3-84BB32FB7675}" name="ID"/>
     <tableColumn id="2" xr3:uid="{D44FAD73-D8DB-4B49-B939-D1640546234B}" name="Description"/>
@@ -491,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +727,7 @@
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
     <col min="2" max="2" width="64.109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="63.21875" customWidth="1"/>
+    <col min="4" max="4" width="67.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
@@ -547,9 +772,6 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -559,10 +781,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -573,10 +792,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -587,29 +803,119 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"partially"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{EF07C501-16C5-42F5-B4B1-8D80038DD3D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{EF07C501-16C5-42F5-B4B1-8D80038DD3D9}">
       <formula1>"yes,partially,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{E9D5AA90-9FA3-427F-A6D2-95229029B874}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11" xr:uid="{E9D5AA90-9FA3-427F-A6D2-95229029B874}">
       <formula1>"low;medium;high"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
init io submodule, and change TennisDataFrame from class to TypeAlias
</commit_message>
<xml_diff>
--- a/to-do.xlsx
+++ b/to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\My Drive (matteopardi2@gmail.com)\Projects\TENNIS - Tennis-Ranking (branch v2.0)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B1E783-DBDF-47A1-BE07-39670DAD114D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03961238-0113-44B3-BC69-B0C57F45AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-7944" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="to-do" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Fai il metodo di ottimizzazione di TennisUniverse</t>
+  </si>
+  <si>
+    <t>t11</t>
+  </si>
+  <si>
+    <t>Controlla che vada tutto ok con installazione python 3.12. Installa tutti I pacchetti (matplotlib…)</t>
   </si>
 </sst>
 </file>
@@ -179,14 +185,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -216,6 +228,9 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -256,11 +271,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}" name="Table1" displayName="Table1" ref="A1:I11" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
-  <autoFilter ref="A1:I11" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}" name="Table1" displayName="Table1" ref="A1:I12" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
+  <autoFilter ref="A1:I12" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
+    <sortCondition ref="F1:F12"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4C27F59C-46C4-4AF8-8CE3-84BB32FB7675}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{D44FAD73-D8DB-4B49-B939-D1640546234B}" name="Description"/>
+    <tableColumn id="2" xr3:uid="{D44FAD73-D8DB-4B49-B939-D1640546234B}" name="Description" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{E24BF007-BA40-4FCD-A331-C8AE56FFB153}" name="Done? [y/p/n]"/>
     <tableColumn id="4" xr3:uid="{8ED4B246-5218-406C-BF8B-830375879A96}" name="Notes"/>
     <tableColumn id="5" xr3:uid="{42BC9D7F-D263-4F99-B9AA-07F8FA3030A9}" name="Priority"/>
@@ -536,16 +554,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="64.109375" customWidth="1"/>
+    <col min="2" max="2" width="64.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="67.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -557,7 +575,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -582,83 +600,95 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C8" t="s">
@@ -667,60 +697,53 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C11">
+  <conditionalFormatting sqref="C2:C12">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"partially"</formula>
     </cfRule>
@@ -732,10 +755,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{EF07C501-16C5-42F5-B4B1-8D80038DD3D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C12" xr:uid="{EF07C501-16C5-42F5-B4B1-8D80038DD3D9}">
       <formula1>"yes,partially,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11" xr:uid="{E9D5AA90-9FA3-427F-A6D2-95229029B874}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E12" xr:uid="{E9D5AA90-9FA3-427F-A6D2-95229029B874}">
       <formula1>"low;medium;high"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add TennisUniverse and fix bug
</commit_message>
<xml_diff>
--- a/to-do.xlsx
+++ b/to-do.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\My Drive (matteopardi2@gmail.com)\Projects\TENNIS - Tennis-Ranking (branch v2.0)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03961238-0113-44B3-BC69-B0C57F45AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E354AB-327E-413D-B0C3-39901A187FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-7944" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Queue</t>
   </si>
   <si>
@@ -66,51 +63,24 @@
     <t>Fai Toringo.py</t>
   </si>
   <si>
-    <t>t1</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>t3</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
     <t>Fai __init__.py di scoring_systems</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>t5</t>
-  </si>
-  <si>
     <t>Fai LogLikelihoodTerm.py</t>
   </si>
   <si>
-    <t>t6</t>
-  </si>
-  <si>
     <t>Fai Loss.py</t>
   </si>
   <si>
-    <t>t7</t>
-  </si>
-  <si>
     <t>Fai TennisDataframe.py</t>
   </si>
   <si>
-    <t>t8</t>
-  </si>
-  <si>
     <t>Intendo la classe derivata da pd.Dataframe… con le colonne già inizializzate</t>
   </si>
   <si>
-    <t>t9</t>
-  </si>
-  <si>
     <t>Fai import_notion_csv.py</t>
   </si>
   <si>
@@ -133,6 +103,33 @@
   </si>
   <si>
     <t>Controlla che vada tutto ok con installazione python 3.12. Installa tutti I pacchetti (matplotlib…)</t>
+  </si>
+  <si>
+    <t>t01</t>
+  </si>
+  <si>
+    <t>t02</t>
+  </si>
+  <si>
+    <t>t03</t>
+  </si>
+  <si>
+    <t>t04</t>
+  </si>
+  <si>
+    <t>t05</t>
+  </si>
+  <si>
+    <t>t06</t>
+  </si>
+  <si>
+    <t>t07</t>
+  </si>
+  <si>
+    <t>t08</t>
+  </si>
+  <si>
+    <t>t09</t>
   </si>
 </sst>
 </file>
@@ -274,7 +271,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}" name="Table1" displayName="Table1" ref="A1:I12" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <autoFilter ref="A1:I12" xr:uid="{61DD4948-91FD-45F2-8B0F-81BFCA7A3FF6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
-    <sortCondition ref="F1:F12"/>
+    <sortCondition ref="A1:A12"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4C27F59C-46C4-4AF8-8CE3-84BB32FB7675}" name="ID"/>
@@ -557,7 +554,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,30 +585,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -619,127 +613,118 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>